<commit_message>
at this point i am going to make the funcudmental unit of this be per experiment, I feel like, agregation logic and the expeimrent manager is just not working.
</commit_message>
<xml_diff>
--- a/metadata/plate_metadata/20250415_well_metadata.xlsx
+++ b/metadata/plate_metadata/20250415_well_metadata.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nick/Cole Trapnell's Lab Dropbox/Nick Lammers/Nick/morphseq/metadata/well_metadata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marazzanocolon/Documents/PhD Folder/morphSeq/YX1_imaging_plates/yes-genotyped/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5C81106-BEF0-4A42-B544-FFDEB7AC9D85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6D375B9-9CE9-CE42-9AD0-417BCE4238A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="17140" activeTab="2" xr2:uid="{1D111BDF-EAD8-A94F-AA28-88CC9649B22F}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="30240" windowHeight="17140" activeTab="8" xr2:uid="{1D111BDF-EAD8-A94F-AA28-88CC9649B22F}"/>
   </bookViews>
   <sheets>
     <sheet name="medium" sheetId="1" r:id="rId1"/>
     <sheet name="mold_type" sheetId="3" r:id="rId2"/>
     <sheet name="genotype" sheetId="4" r:id="rId3"/>
-    <sheet name="chem_perturbation" sheetId="5" r:id="rId4"/>
-    <sheet name="start_age_hpf" sheetId="6" r:id="rId5"/>
-    <sheet name="series_number_map" sheetId="9" r:id="rId6"/>
-    <sheet name="start_age_morph" sheetId="8" r:id="rId7"/>
-    <sheet name="embryos_per_well" sheetId="7" r:id="rId8"/>
+    <sheet name="start_age_hpf" sheetId="6" r:id="rId4"/>
+    <sheet name="series_number_map" sheetId="9" r:id="rId5"/>
+    <sheet name="start_age_morph" sheetId="8" r:id="rId6"/>
+    <sheet name="embryos_per_well" sheetId="7" r:id="rId7"/>
+    <sheet name="chem_perturbation" sheetId="5" r:id="rId8"/>
+    <sheet name="temperature" sheetId="15" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="13">
   <si>
     <t>A</t>
   </si>
@@ -72,20 +73,23 @@
     <t>None</t>
   </si>
   <si>
-    <t>MC1</t>
+    <t>MC05</t>
   </si>
   <si>
-    <t>EM</t>
+    <t>tbd cep290s</t>
   </si>
   <si>
-    <t>MC05</t>
+    <t>cep290_unkown</t>
+  </si>
+  <si>
+    <t>failed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -106,6 +110,19 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -124,16 +141,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{EED4C45B-E532-9A47-8954-E433DAA4E196}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -448,7 +468,7 @@
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M4" sqref="A4:M9"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -496,28 +516,28 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="J2" t="s">
         <v>9</v>
@@ -537,28 +557,28 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="J3" t="s">
         <v>9</v>
@@ -578,28 +598,28 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="J4" t="s">
         <v>9</v>
@@ -619,28 +639,28 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I5" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="J5" t="s">
         <v>9</v>
@@ -660,28 +680,28 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="J6" t="s">
         <v>9</v>
@@ -701,28 +721,28 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I7" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="J7" t="s">
         <v>9</v>
@@ -742,28 +762,28 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I8" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="J8" t="s">
         <v>9</v>
@@ -783,28 +803,28 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="G9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="H9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="I9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="J9" t="s">
         <v>9</v>
@@ -820,6 +840,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1207,10 +1228,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C77E54D0-3682-084C-87D6-317C30F3BB42}">
-  <dimension ref="A1:M9"/>
+  <dimension ref="A1:M11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1257,137 +1278,343 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M6" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
+      <c r="B7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M7" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="2"/>
+      <c r="B8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="2"/>
+      <c r="B9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <f>SUM(C1:C10)</f>
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1396,7 +1623,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB6F99FE-D096-1C40-A0AC-66A53996EA64}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9F11C58-0A1C-8F4D-A690-43B3ED108271}">
   <dimension ref="A1:M9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1447,328 +1674,328 @@
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K2" t="s">
-        <v>8</v>
-      </c>
-      <c r="L2" t="s">
-        <v>8</v>
-      </c>
-      <c r="M2" t="s">
-        <v>8</v>
+      <c r="B2">
+        <v>12</v>
+      </c>
+      <c r="C2">
+        <v>12</v>
+      </c>
+      <c r="D2">
+        <v>12</v>
+      </c>
+      <c r="E2">
+        <v>12</v>
+      </c>
+      <c r="F2">
+        <v>12</v>
+      </c>
+      <c r="G2">
+        <v>12</v>
+      </c>
+      <c r="H2">
+        <v>12</v>
+      </c>
+      <c r="I2">
+        <v>12</v>
+      </c>
+      <c r="J2">
+        <v>12</v>
+      </c>
+      <c r="K2">
+        <v>12</v>
+      </c>
+      <c r="L2">
+        <v>12</v>
+      </c>
+      <c r="M2">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>8</v>
-      </c>
-      <c r="F3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H3" t="s">
-        <v>8</v>
-      </c>
-      <c r="I3" t="s">
-        <v>8</v>
-      </c>
-      <c r="J3" t="s">
-        <v>8</v>
-      </c>
-      <c r="K3" t="s">
-        <v>8</v>
-      </c>
-      <c r="L3" t="s">
-        <v>8</v>
-      </c>
-      <c r="M3" t="s">
-        <v>8</v>
+      <c r="B3">
+        <v>12</v>
+      </c>
+      <c r="C3">
+        <v>12</v>
+      </c>
+      <c r="D3">
+        <v>12</v>
+      </c>
+      <c r="E3">
+        <v>12</v>
+      </c>
+      <c r="F3">
+        <v>12</v>
+      </c>
+      <c r="G3">
+        <v>12</v>
+      </c>
+      <c r="H3">
+        <v>12</v>
+      </c>
+      <c r="I3">
+        <v>12</v>
+      </c>
+      <c r="J3">
+        <v>12</v>
+      </c>
+      <c r="K3">
+        <v>12</v>
+      </c>
+      <c r="L3">
+        <v>12</v>
+      </c>
+      <c r="M3">
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F4" t="s">
-        <v>8</v>
-      </c>
-      <c r="G4" t="s">
-        <v>8</v>
-      </c>
-      <c r="H4" t="s">
-        <v>8</v>
-      </c>
-      <c r="I4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J4" t="s">
-        <v>8</v>
-      </c>
-      <c r="K4" t="s">
-        <v>8</v>
-      </c>
-      <c r="L4" t="s">
-        <v>8</v>
-      </c>
-      <c r="M4" t="s">
-        <v>8</v>
+      <c r="B4">
+        <v>12</v>
+      </c>
+      <c r="C4">
+        <v>12</v>
+      </c>
+      <c r="D4">
+        <v>12</v>
+      </c>
+      <c r="E4">
+        <v>12</v>
+      </c>
+      <c r="F4">
+        <v>12</v>
+      </c>
+      <c r="G4">
+        <v>12</v>
+      </c>
+      <c r="H4">
+        <v>12</v>
+      </c>
+      <c r="I4">
+        <v>12</v>
+      </c>
+      <c r="J4">
+        <v>12</v>
+      </c>
+      <c r="K4">
+        <v>12</v>
+      </c>
+      <c r="L4">
+        <v>12</v>
+      </c>
+      <c r="M4">
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
-      <c r="B5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" t="s">
-        <v>8</v>
-      </c>
-      <c r="F5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G5" t="s">
-        <v>8</v>
-      </c>
-      <c r="H5" t="s">
-        <v>8</v>
-      </c>
-      <c r="I5" t="s">
-        <v>8</v>
-      </c>
-      <c r="J5" t="s">
-        <v>8</v>
-      </c>
-      <c r="K5" t="s">
-        <v>8</v>
-      </c>
-      <c r="L5" t="s">
-        <v>8</v>
-      </c>
-      <c r="M5" t="s">
-        <v>8</v>
+      <c r="B5">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>12</v>
+      </c>
+      <c r="D5">
+        <v>12</v>
+      </c>
+      <c r="E5">
+        <v>12</v>
+      </c>
+      <c r="F5">
+        <v>12</v>
+      </c>
+      <c r="G5">
+        <v>12</v>
+      </c>
+      <c r="H5">
+        <v>12</v>
+      </c>
+      <c r="I5">
+        <v>12</v>
+      </c>
+      <c r="J5">
+        <v>12</v>
+      </c>
+      <c r="K5">
+        <v>12</v>
+      </c>
+      <c r="L5">
+        <v>12</v>
+      </c>
+      <c r="M5">
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" t="s">
-        <v>8</v>
-      </c>
-      <c r="G6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I6" t="s">
-        <v>8</v>
-      </c>
-      <c r="J6" t="s">
-        <v>8</v>
-      </c>
-      <c r="K6" t="s">
-        <v>8</v>
-      </c>
-      <c r="L6" t="s">
-        <v>8</v>
-      </c>
-      <c r="M6" t="s">
-        <v>8</v>
+      <c r="B6">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>12</v>
+      </c>
+      <c r="D6">
+        <v>12</v>
+      </c>
+      <c r="E6">
+        <v>12</v>
+      </c>
+      <c r="F6">
+        <v>12</v>
+      </c>
+      <c r="G6">
+        <v>12</v>
+      </c>
+      <c r="H6">
+        <v>12</v>
+      </c>
+      <c r="I6">
+        <v>12</v>
+      </c>
+      <c r="J6">
+        <v>12</v>
+      </c>
+      <c r="K6">
+        <v>12</v>
+      </c>
+      <c r="L6">
+        <v>12</v>
+      </c>
+      <c r="M6">
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" t="s">
-        <v>8</v>
-      </c>
-      <c r="G7" t="s">
-        <v>8</v>
-      </c>
-      <c r="H7" t="s">
-        <v>8</v>
-      </c>
-      <c r="I7" t="s">
-        <v>8</v>
-      </c>
-      <c r="J7" t="s">
-        <v>8</v>
-      </c>
-      <c r="K7" t="s">
-        <v>8</v>
-      </c>
-      <c r="L7" t="s">
-        <v>8</v>
-      </c>
-      <c r="M7" t="s">
-        <v>8</v>
+      <c r="B7">
+        <v>12</v>
+      </c>
+      <c r="C7">
+        <v>12</v>
+      </c>
+      <c r="D7">
+        <v>12</v>
+      </c>
+      <c r="E7">
+        <v>12</v>
+      </c>
+      <c r="F7">
+        <v>12</v>
+      </c>
+      <c r="G7">
+        <v>12</v>
+      </c>
+      <c r="H7">
+        <v>12</v>
+      </c>
+      <c r="I7">
+        <v>12</v>
+      </c>
+      <c r="J7">
+        <v>12</v>
+      </c>
+      <c r="K7">
+        <v>12</v>
+      </c>
+      <c r="L7">
+        <v>12</v>
+      </c>
+      <c r="M7">
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C8" t="s">
-        <v>8</v>
-      </c>
-      <c r="D8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E8" t="s">
-        <v>8</v>
-      </c>
-      <c r="F8" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" t="s">
-        <v>8</v>
-      </c>
-      <c r="H8" t="s">
-        <v>8</v>
-      </c>
-      <c r="I8" t="s">
-        <v>8</v>
-      </c>
-      <c r="J8" t="s">
-        <v>8</v>
-      </c>
-      <c r="K8" t="s">
-        <v>8</v>
-      </c>
-      <c r="L8" t="s">
-        <v>8</v>
-      </c>
-      <c r="M8" t="s">
-        <v>8</v>
+      <c r="B8">
+        <v>12</v>
+      </c>
+      <c r="C8">
+        <v>12</v>
+      </c>
+      <c r="D8">
+        <v>12</v>
+      </c>
+      <c r="E8">
+        <v>12</v>
+      </c>
+      <c r="F8">
+        <v>12</v>
+      </c>
+      <c r="G8">
+        <v>12</v>
+      </c>
+      <c r="H8">
+        <v>12</v>
+      </c>
+      <c r="I8">
+        <v>12</v>
+      </c>
+      <c r="J8">
+        <v>12</v>
+      </c>
+      <c r="K8">
+        <v>12</v>
+      </c>
+      <c r="L8">
+        <v>12</v>
+      </c>
+      <c r="M8">
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
-      <c r="B9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" t="s">
-        <v>8</v>
-      </c>
-      <c r="E9" t="s">
-        <v>8</v>
-      </c>
-      <c r="F9" t="s">
-        <v>8</v>
-      </c>
-      <c r="G9" t="s">
-        <v>8</v>
-      </c>
-      <c r="H9" t="s">
-        <v>8</v>
-      </c>
-      <c r="I9" t="s">
-        <v>8</v>
-      </c>
-      <c r="J9" t="s">
-        <v>8</v>
-      </c>
-      <c r="K9" t="s">
-        <v>8</v>
-      </c>
-      <c r="L9" t="s">
-        <v>8</v>
-      </c>
-      <c r="M9" t="s">
-        <v>8</v>
+      <c r="B9">
+        <v>12</v>
+      </c>
+      <c r="C9">
+        <v>12</v>
+      </c>
+      <c r="D9">
+        <v>12</v>
+      </c>
+      <c r="E9">
+        <v>12</v>
+      </c>
+      <c r="F9">
+        <v>12</v>
+      </c>
+      <c r="G9">
+        <v>12</v>
+      </c>
+      <c r="H9">
+        <v>12</v>
+      </c>
+      <c r="I9">
+        <v>12</v>
+      </c>
+      <c r="J9">
+        <v>12</v>
+      </c>
+      <c r="K9">
+        <v>12</v>
+      </c>
+      <c r="L9">
+        <v>12</v>
+      </c>
+      <c r="M9">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1777,387 +2004,6 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9F11C58-0A1C-8F4D-A690-43B3ED108271}">
-  <dimension ref="A1:M9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B1">
-        <v>1</v>
-      </c>
-      <c r="C1">
-        <v>2</v>
-      </c>
-      <c r="D1">
-        <v>3</v>
-      </c>
-      <c r="E1">
-        <v>4</v>
-      </c>
-      <c r="F1">
-        <v>5</v>
-      </c>
-      <c r="G1">
-        <v>6</v>
-      </c>
-      <c r="H1">
-        <v>7</v>
-      </c>
-      <c r="I1">
-        <v>8</v>
-      </c>
-      <c r="J1">
-        <v>9</v>
-      </c>
-      <c r="K1">
-        <v>10</v>
-      </c>
-      <c r="L1">
-        <v>11</v>
-      </c>
-      <c r="M1">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>12</v>
-      </c>
-      <c r="C2">
-        <v>12</v>
-      </c>
-      <c r="D2">
-        <v>12</v>
-      </c>
-      <c r="E2">
-        <v>12</v>
-      </c>
-      <c r="F2">
-        <v>12</v>
-      </c>
-      <c r="G2">
-        <v>12</v>
-      </c>
-      <c r="H2">
-        <v>12</v>
-      </c>
-      <c r="I2">
-        <v>12</v>
-      </c>
-      <c r="J2">
-        <v>12</v>
-      </c>
-      <c r="K2">
-        <v>12</v>
-      </c>
-      <c r="L2">
-        <v>12</v>
-      </c>
-      <c r="M2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>12</v>
-      </c>
-      <c r="C3">
-        <v>12</v>
-      </c>
-      <c r="D3">
-        <v>12</v>
-      </c>
-      <c r="E3">
-        <v>12</v>
-      </c>
-      <c r="F3">
-        <v>12</v>
-      </c>
-      <c r="G3">
-        <v>12</v>
-      </c>
-      <c r="H3">
-        <v>12</v>
-      </c>
-      <c r="I3">
-        <v>12</v>
-      </c>
-      <c r="J3">
-        <v>12</v>
-      </c>
-      <c r="K3">
-        <v>12</v>
-      </c>
-      <c r="L3">
-        <v>12</v>
-      </c>
-      <c r="M3">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>12</v>
-      </c>
-      <c r="C4">
-        <v>12</v>
-      </c>
-      <c r="D4">
-        <v>12</v>
-      </c>
-      <c r="E4">
-        <v>12</v>
-      </c>
-      <c r="F4">
-        <v>12</v>
-      </c>
-      <c r="G4">
-        <v>12</v>
-      </c>
-      <c r="H4">
-        <v>12</v>
-      </c>
-      <c r="I4">
-        <v>12</v>
-      </c>
-      <c r="J4">
-        <v>12</v>
-      </c>
-      <c r="K4">
-        <v>12</v>
-      </c>
-      <c r="L4">
-        <v>12</v>
-      </c>
-      <c r="M4">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5">
-        <v>12</v>
-      </c>
-      <c r="C5">
-        <v>12</v>
-      </c>
-      <c r="D5">
-        <v>12</v>
-      </c>
-      <c r="E5">
-        <v>12</v>
-      </c>
-      <c r="F5">
-        <v>12</v>
-      </c>
-      <c r="G5">
-        <v>12</v>
-      </c>
-      <c r="H5">
-        <v>12</v>
-      </c>
-      <c r="I5">
-        <v>12</v>
-      </c>
-      <c r="J5">
-        <v>12</v>
-      </c>
-      <c r="K5">
-        <v>12</v>
-      </c>
-      <c r="L5">
-        <v>12</v>
-      </c>
-      <c r="M5">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>12</v>
-      </c>
-      <c r="C6">
-        <v>12</v>
-      </c>
-      <c r="D6">
-        <v>12</v>
-      </c>
-      <c r="E6">
-        <v>12</v>
-      </c>
-      <c r="F6">
-        <v>12</v>
-      </c>
-      <c r="G6">
-        <v>12</v>
-      </c>
-      <c r="H6">
-        <v>12</v>
-      </c>
-      <c r="I6">
-        <v>12</v>
-      </c>
-      <c r="J6">
-        <v>12</v>
-      </c>
-      <c r="K6">
-        <v>12</v>
-      </c>
-      <c r="L6">
-        <v>12</v>
-      </c>
-      <c r="M6">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>12</v>
-      </c>
-      <c r="C7">
-        <v>12</v>
-      </c>
-      <c r="D7">
-        <v>12</v>
-      </c>
-      <c r="E7">
-        <v>12</v>
-      </c>
-      <c r="F7">
-        <v>12</v>
-      </c>
-      <c r="G7">
-        <v>12</v>
-      </c>
-      <c r="H7">
-        <v>12</v>
-      </c>
-      <c r="I7">
-        <v>12</v>
-      </c>
-      <c r="J7">
-        <v>12</v>
-      </c>
-      <c r="K7">
-        <v>12</v>
-      </c>
-      <c r="L7">
-        <v>12</v>
-      </c>
-      <c r="M7">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8">
-        <v>12</v>
-      </c>
-      <c r="C8">
-        <v>12</v>
-      </c>
-      <c r="D8">
-        <v>12</v>
-      </c>
-      <c r="E8">
-        <v>12</v>
-      </c>
-      <c r="F8">
-        <v>12</v>
-      </c>
-      <c r="G8">
-        <v>12</v>
-      </c>
-      <c r="H8">
-        <v>12</v>
-      </c>
-      <c r="I8">
-        <v>12</v>
-      </c>
-      <c r="J8">
-        <v>12</v>
-      </c>
-      <c r="K8">
-        <v>12</v>
-      </c>
-      <c r="L8">
-        <v>12</v>
-      </c>
-      <c r="M8">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>7</v>
-      </c>
-      <c r="B9">
-        <v>12</v>
-      </c>
-      <c r="C9">
-        <v>12</v>
-      </c>
-      <c r="D9">
-        <v>12</v>
-      </c>
-      <c r="E9">
-        <v>12</v>
-      </c>
-      <c r="F9">
-        <v>12</v>
-      </c>
-      <c r="G9">
-        <v>12</v>
-      </c>
-      <c r="H9">
-        <v>12</v>
-      </c>
-      <c r="I9">
-        <v>12</v>
-      </c>
-      <c r="J9">
-        <v>12</v>
-      </c>
-      <c r="K9">
-        <v>12</v>
-      </c>
-      <c r="L9">
-        <v>12</v>
-      </c>
-      <c r="M9">
-        <v>12</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D46C1C09-F499-E742-B6FA-2A1DD3DA1E07}">
   <dimension ref="A1:M9"/>
   <sheetViews>
@@ -2226,28 +2072,28 @@
         <v>33</v>
       </c>
       <c r="G2" s="1">
-        <f t="shared" ref="G2:G8" si="0">G3+1</f>
+        <f t="shared" ref="G2:G7" si="0">G3+1</f>
         <v>48</v>
       </c>
       <c r="H2" s="1">
         <v>49</v>
       </c>
       <c r="I2" s="1">
-        <f t="shared" ref="I2:I8" si="1">I3+1</f>
+        <f t="shared" ref="I2:I7" si="1">I3+1</f>
         <v>64</v>
       </c>
       <c r="J2" s="1">
         <v>65</v>
       </c>
       <c r="K2" s="1">
-        <f t="shared" ref="K2:K8" si="2">K3+1</f>
+        <f t="shared" ref="K2:K7" si="2">K3+1</f>
         <v>80</v>
       </c>
       <c r="L2" s="1">
         <v>81</v>
       </c>
       <c r="M2" s="1">
-        <f t="shared" ref="M2:M8" si="3">M3+1</f>
+        <f t="shared" ref="M2:M7" si="3">M3+1</f>
         <v>96</v>
       </c>
     </row>
@@ -2593,7 +2439,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58C580E4-EBDF-214A-AF19-4A9B46AB72D0}">
   <dimension ref="A1:M9"/>
   <sheetViews>
@@ -2686,7 +2532,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{84CF5125-30A0-D544-A1A7-3583E3A1F38E}">
   <dimension ref="A1:M9"/>
   <sheetViews>
@@ -2777,4 +2623,769 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB6F99FE-D096-1C40-A0AC-66A53996EA64}">
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R28" sqref="R28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B1">
+        <v>1</v>
+      </c>
+      <c r="C1">
+        <v>2</v>
+      </c>
+      <c r="D1">
+        <v>3</v>
+      </c>
+      <c r="E1">
+        <v>4</v>
+      </c>
+      <c r="F1">
+        <v>5</v>
+      </c>
+      <c r="G1">
+        <v>6</v>
+      </c>
+      <c r="H1">
+        <v>7</v>
+      </c>
+      <c r="I1">
+        <v>8</v>
+      </c>
+      <c r="J1">
+        <v>9</v>
+      </c>
+      <c r="K1">
+        <v>10</v>
+      </c>
+      <c r="L1">
+        <v>11</v>
+      </c>
+      <c r="M1">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" t="s">
+        <v>8</v>
+      </c>
+      <c r="K2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I3" t="s">
+        <v>8</v>
+      </c>
+      <c r="J3" t="s">
+        <v>8</v>
+      </c>
+      <c r="K3" t="s">
+        <v>8</v>
+      </c>
+      <c r="L3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>8</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" t="s">
+        <v>8</v>
+      </c>
+      <c r="K4" t="s">
+        <v>8</v>
+      </c>
+      <c r="L4" t="s">
+        <v>8</v>
+      </c>
+      <c r="M4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" t="s">
+        <v>8</v>
+      </c>
+      <c r="I5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K5" t="s">
+        <v>8</v>
+      </c>
+      <c r="L5" t="s">
+        <v>8</v>
+      </c>
+      <c r="M5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" t="s">
+        <v>8</v>
+      </c>
+      <c r="I6" t="s">
+        <v>8</v>
+      </c>
+      <c r="J6" t="s">
+        <v>8</v>
+      </c>
+      <c r="K6" t="s">
+        <v>8</v>
+      </c>
+      <c r="L6" t="s">
+        <v>8</v>
+      </c>
+      <c r="M6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" t="s">
+        <v>8</v>
+      </c>
+      <c r="I7" t="s">
+        <v>8</v>
+      </c>
+      <c r="J7" t="s">
+        <v>8</v>
+      </c>
+      <c r="K7" t="s">
+        <v>8</v>
+      </c>
+      <c r="L7" t="s">
+        <v>8</v>
+      </c>
+      <c r="M7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" t="s">
+        <v>8</v>
+      </c>
+      <c r="J8" t="s">
+        <v>8</v>
+      </c>
+      <c r="K8" t="s">
+        <v>8</v>
+      </c>
+      <c r="L8" t="s">
+        <v>8</v>
+      </c>
+      <c r="M8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D9" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" t="s">
+        <v>8</v>
+      </c>
+      <c r="F9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G9" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" t="s">
+        <v>8</v>
+      </c>
+      <c r="I9" t="s">
+        <v>8</v>
+      </c>
+      <c r="J9" t="s">
+        <v>8</v>
+      </c>
+      <c r="K9" t="s">
+        <v>8</v>
+      </c>
+      <c r="L9" t="s">
+        <v>8</v>
+      </c>
+      <c r="M9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B70EF86B-8022-C74B-A47C-4860A5B03C79}">
+  <dimension ref="A1:M9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K14" sqref="K14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="10.83203125" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B1" s="3">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3">
+        <v>4</v>
+      </c>
+      <c r="F1" s="3">
+        <v>5</v>
+      </c>
+      <c r="G1" s="3">
+        <v>6</v>
+      </c>
+      <c r="H1" s="3">
+        <v>7</v>
+      </c>
+      <c r="I1" s="3">
+        <v>8</v>
+      </c>
+      <c r="J1" s="3">
+        <v>9</v>
+      </c>
+      <c r="K1" s="3">
+        <v>10</v>
+      </c>
+      <c r="L1" s="3">
+        <v>11</v>
+      </c>
+      <c r="M1" s="3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3">
+        <v>30</v>
+      </c>
+      <c r="C2" s="3">
+        <v>30</v>
+      </c>
+      <c r="D2" s="3">
+        <v>30</v>
+      </c>
+      <c r="E2" s="3">
+        <v>30</v>
+      </c>
+      <c r="F2" s="3">
+        <v>30</v>
+      </c>
+      <c r="G2" s="3">
+        <v>30</v>
+      </c>
+      <c r="H2" s="3">
+        <v>30</v>
+      </c>
+      <c r="I2" s="3">
+        <v>30</v>
+      </c>
+      <c r="J2" s="3">
+        <v>30</v>
+      </c>
+      <c r="K2" s="3">
+        <v>30</v>
+      </c>
+      <c r="L2" s="3">
+        <v>30</v>
+      </c>
+      <c r="M2" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3">
+        <v>30</v>
+      </c>
+      <c r="C3" s="3">
+        <v>30</v>
+      </c>
+      <c r="D3" s="3">
+        <v>30</v>
+      </c>
+      <c r="E3" s="3">
+        <v>30</v>
+      </c>
+      <c r="F3" s="3">
+        <v>30</v>
+      </c>
+      <c r="G3" s="3">
+        <v>30</v>
+      </c>
+      <c r="H3" s="3">
+        <v>30</v>
+      </c>
+      <c r="I3" s="3">
+        <v>30</v>
+      </c>
+      <c r="J3" s="3">
+        <v>30</v>
+      </c>
+      <c r="K3" s="3">
+        <v>30</v>
+      </c>
+      <c r="L3" s="3">
+        <v>30</v>
+      </c>
+      <c r="M3" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3">
+        <v>30</v>
+      </c>
+      <c r="C4" s="3">
+        <v>30</v>
+      </c>
+      <c r="D4" s="3">
+        <v>30</v>
+      </c>
+      <c r="E4" s="3">
+        <v>30</v>
+      </c>
+      <c r="F4" s="3">
+        <v>30</v>
+      </c>
+      <c r="G4" s="3">
+        <v>30</v>
+      </c>
+      <c r="H4" s="3">
+        <v>30</v>
+      </c>
+      <c r="I4" s="3">
+        <v>30</v>
+      </c>
+      <c r="J4" s="3">
+        <v>30</v>
+      </c>
+      <c r="K4" s="3">
+        <v>30</v>
+      </c>
+      <c r="L4" s="3">
+        <v>30</v>
+      </c>
+      <c r="M4" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3">
+        <v>30</v>
+      </c>
+      <c r="C5" s="3">
+        <v>30</v>
+      </c>
+      <c r="D5" s="3">
+        <v>30</v>
+      </c>
+      <c r="E5" s="3">
+        <v>30</v>
+      </c>
+      <c r="F5" s="3">
+        <v>30</v>
+      </c>
+      <c r="G5" s="3">
+        <v>30</v>
+      </c>
+      <c r="H5" s="3">
+        <v>30</v>
+      </c>
+      <c r="I5" s="3">
+        <v>30</v>
+      </c>
+      <c r="J5" s="3">
+        <v>30</v>
+      </c>
+      <c r="K5" s="3">
+        <v>30</v>
+      </c>
+      <c r="L5" s="3">
+        <v>30</v>
+      </c>
+      <c r="M5" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3">
+        <v>30</v>
+      </c>
+      <c r="C6" s="3">
+        <v>30</v>
+      </c>
+      <c r="D6" s="3">
+        <v>30</v>
+      </c>
+      <c r="E6" s="3">
+        <v>30</v>
+      </c>
+      <c r="F6" s="3">
+        <v>30</v>
+      </c>
+      <c r="G6" s="3">
+        <v>30</v>
+      </c>
+      <c r="H6" s="3">
+        <v>30</v>
+      </c>
+      <c r="I6" s="3">
+        <v>30</v>
+      </c>
+      <c r="J6" s="3">
+        <v>30</v>
+      </c>
+      <c r="K6" s="3">
+        <v>30</v>
+      </c>
+      <c r="L6" s="3">
+        <v>30</v>
+      </c>
+      <c r="M6" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3">
+        <v>30</v>
+      </c>
+      <c r="C7" s="3">
+        <v>30</v>
+      </c>
+      <c r="D7" s="3">
+        <v>30</v>
+      </c>
+      <c r="E7" s="3">
+        <v>30</v>
+      </c>
+      <c r="F7" s="3">
+        <v>30</v>
+      </c>
+      <c r="G7" s="3">
+        <v>30</v>
+      </c>
+      <c r="H7" s="3">
+        <v>30</v>
+      </c>
+      <c r="I7" s="3">
+        <v>30</v>
+      </c>
+      <c r="J7" s="3">
+        <v>30</v>
+      </c>
+      <c r="K7" s="3">
+        <v>30</v>
+      </c>
+      <c r="L7" s="3">
+        <v>30</v>
+      </c>
+      <c r="M7" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3">
+        <v>30</v>
+      </c>
+      <c r="C8" s="3">
+        <v>30</v>
+      </c>
+      <c r="D8" s="3">
+        <v>30</v>
+      </c>
+      <c r="E8" s="3">
+        <v>30</v>
+      </c>
+      <c r="F8" s="3">
+        <v>30</v>
+      </c>
+      <c r="G8" s="3">
+        <v>30</v>
+      </c>
+      <c r="H8" s="3">
+        <v>30</v>
+      </c>
+      <c r="I8" s="3">
+        <v>30</v>
+      </c>
+      <c r="J8" s="3">
+        <v>30</v>
+      </c>
+      <c r="K8" s="3">
+        <v>30</v>
+      </c>
+      <c r="L8" s="3">
+        <v>30</v>
+      </c>
+      <c r="M8" s="3">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3">
+        <v>30</v>
+      </c>
+      <c r="C9" s="3">
+        <v>30</v>
+      </c>
+      <c r="D9" s="3">
+        <v>30</v>
+      </c>
+      <c r="E9" s="3">
+        <v>30</v>
+      </c>
+      <c r="F9" s="3">
+        <v>30</v>
+      </c>
+      <c r="G9" s="3">
+        <v>30</v>
+      </c>
+      <c r="H9" s="3">
+        <v>30</v>
+      </c>
+      <c r="I9" s="3">
+        <v>30</v>
+      </c>
+      <c r="J9" s="3">
+        <v>30</v>
+      </c>
+      <c r="K9" s="3">
+        <v>30</v>
+      </c>
+      <c r="L9" s="3">
+        <v>30</v>
+      </c>
+      <c r="M9" s="3">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>